<commit_message>
testes de alocação mal sucedidos
</commit_message>
<xml_diff>
--- a/src/Escala ASO1 - Central - Julho.xlsx
+++ b/src/Escala ASO1 - Central - Julho.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>Escala ASO1 - Central - Julho</t>
   </si>
@@ -51,9 +51,6 @@
     <t>B2</t>
   </si>
   <si>
-    <t>Q2</t>
-  </si>
-  <si>
     <t>B1</t>
   </si>
   <si>
@@ -64,6 +61,12 @@
   </si>
   <si>
     <t>Zeze</t>
+  </si>
+  <si>
+    <t>Tata</t>
+  </si>
+  <si>
+    <t>Tretas</t>
   </si>
 </sst>
 </file>
@@ -667,7 +670,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -682,31 +685,31 @@
         <v>11</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="3" t="s">
-        <v>11</v>
+      <c r="N4" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>9</v>
@@ -718,60 +721,60 @@
         <v>8</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="W4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AC4" s="3" t="s">
-        <v>10</v>
+      <c r="AC4" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="AD4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AG4" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row customHeight="1" ht="20" r="5" spans="1:33">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -780,28 +783,28 @@
         <v>11</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>8</v>
@@ -816,325 +819,361 @@
         <v>11</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="W5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="X5" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="Y5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AA5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AB5" s="3" t="s">
-        <v>9</v>
+      <c r="AB5" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="AC5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="AD5" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AF5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AG5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row customHeight="1" ht="20" r="6" spans="1:33">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="V6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="W6" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="X6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Y6" s="2" t="s">
-        <v>8</v>
+      <c r="Y6" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="Z6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AA6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB6" s="3" t="s">
-        <v>10</v>
+      <c r="AA6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AF6" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AG6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row customHeight="1" ht="20" r="7" spans="1:33">
       <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s"/>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="3" t="s"/>
+      <c r="G7" s="3" t="s"/>
+      <c r="H7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="3" t="s"/>
+      <c r="K7" s="3" t="s"/>
+      <c r="L7" s="3" t="s"/>
+      <c r="M7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P7" s="3" t="s"/>
+      <c r="Q7" s="3" t="s"/>
+      <c r="R7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T7" s="3" t="s"/>
+      <c r="U7" s="3" t="s"/>
+      <c r="V7" s="3" t="s"/>
+      <c r="W7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z7" s="3" t="s"/>
+      <c r="AA7" s="3" t="s"/>
+      <c r="AB7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE7" s="3" t="s"/>
+      <c r="AF7" s="3" t="s"/>
+      <c r="AG7" s="3" t="s"/>
+    </row>
+    <row customHeight="1" ht="20" r="8" spans="1:33">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="S7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="T7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="V7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="W7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="X7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG7" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="20" r="8" spans="1:33">
-      <c r="A8" s="1" t="n"/>
-      <c r="B8" s="1" t="n"/>
-      <c r="C8" s="3" t="n"/>
-      <c r="D8" s="3" t="n"/>
-      <c r="E8" s="3" t="n"/>
-      <c r="F8" s="3" t="n"/>
-      <c r="G8" s="3" t="n"/>
-      <c r="H8" s="3" t="n"/>
-      <c r="I8" s="3" t="n"/>
-      <c r="J8" s="3" t="n"/>
-      <c r="K8" s="3" t="n"/>
-      <c r="L8" s="3" t="n"/>
-      <c r="M8" s="3" t="n"/>
-      <c r="N8" s="3" t="n"/>
-      <c r="O8" s="3" t="n"/>
-      <c r="P8" s="3" t="n"/>
-      <c r="Q8" s="3" t="n"/>
-      <c r="R8" s="3" t="n"/>
-      <c r="S8" s="3" t="n"/>
-      <c r="T8" s="3" t="n"/>
-      <c r="U8" s="3" t="n"/>
-      <c r="V8" s="3" t="n"/>
-      <c r="W8" s="3" t="n"/>
-      <c r="X8" s="3" t="n"/>
-      <c r="Y8" s="3" t="n"/>
-      <c r="Z8" s="3" t="n"/>
-      <c r="AA8" s="3" t="n"/>
-      <c r="AB8" s="3" t="n"/>
-      <c r="AC8" s="3" t="n"/>
-      <c r="AD8" s="3" t="n"/>
-      <c r="AE8" s="3" t="n"/>
-      <c r="AF8" s="3" t="n"/>
-      <c r="AG8" s="3" t="n"/>
+      <c r="B8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s"/>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="3" t="s"/>
+      <c r="G8" s="3" t="s"/>
+      <c r="H8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="3" t="s"/>
+      <c r="K8" s="3" t="s"/>
+      <c r="L8" s="3" t="s"/>
+      <c r="M8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P8" s="3" t="s"/>
+      <c r="Q8" s="3" t="s"/>
+      <c r="R8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T8" s="3" t="s"/>
+      <c r="U8" s="3" t="s"/>
+      <c r="V8" s="3" t="s"/>
+      <c r="W8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z8" s="3" t="s"/>
+      <c r="AA8" s="3" t="s"/>
+      <c r="AB8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE8" s="3" t="s"/>
+      <c r="AF8" s="3" t="s"/>
+      <c r="AG8" s="3" t="s"/>
     </row>
     <row customHeight="1" ht="20" r="9" spans="1:33">
-      <c r="A9" s="1" t="n"/>
-      <c r="B9" s="1" t="n"/>
-      <c r="C9" s="3" t="n"/>
-      <c r="D9" s="3" t="n"/>
-      <c r="E9" s="3" t="n"/>
-      <c r="F9" s="3" t="n"/>
-      <c r="G9" s="3" t="n"/>
-      <c r="H9" s="3" t="n"/>
-      <c r="I9" s="3" t="n"/>
-      <c r="J9" s="3" t="n"/>
-      <c r="K9" s="3" t="n"/>
-      <c r="L9" s="3" t="n"/>
-      <c r="M9" s="3" t="n"/>
-      <c r="N9" s="3" t="n"/>
-      <c r="O9" s="3" t="n"/>
-      <c r="P9" s="3" t="n"/>
-      <c r="Q9" s="3" t="n"/>
-      <c r="R9" s="3" t="n"/>
-      <c r="S9" s="3" t="n"/>
-      <c r="T9" s="3" t="n"/>
-      <c r="U9" s="3" t="n"/>
-      <c r="V9" s="3" t="n"/>
-      <c r="W9" s="3" t="n"/>
-      <c r="X9" s="3" t="n"/>
-      <c r="Y9" s="3" t="n"/>
-      <c r="Z9" s="3" t="n"/>
-      <c r="AA9" s="3" t="n"/>
-      <c r="AB9" s="3" t="n"/>
-      <c r="AC9" s="3" t="n"/>
-      <c r="AD9" s="3" t="n"/>
-      <c r="AE9" s="3" t="n"/>
-      <c r="AF9" s="3" t="n"/>
-      <c r="AG9" s="3" t="n"/>
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3" t="s"/>
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="3" t="s"/>
+      <c r="G9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="3" t="s"/>
+      <c r="J9" s="3" t="s"/>
+      <c r="K9" s="3" t="s"/>
+      <c r="L9" s="3" t="s"/>
+      <c r="M9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O9" s="3" t="s"/>
+      <c r="P9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q9" s="3" t="s"/>
+      <c r="R9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T9" s="3" t="s"/>
+      <c r="U9" s="3" t="s"/>
+      <c r="V9" s="3" t="s"/>
+      <c r="W9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z9" s="3" t="s"/>
+      <c r="AA9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC9" s="3" t="s"/>
+      <c r="AD9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE9" s="3" t="s"/>
+      <c r="AF9" s="3" t="s"/>
+      <c r="AG9" s="3" t="s"/>
     </row>
     <row customHeight="1" ht="20" r="10" spans="1:33">
       <c r="A10" s="1" t="n"/>

</xml_diff>